<commit_message>
HOPE study modifications for female clients
</commit_message>
<xml_diff>
--- a/app/tables/femaleClients/forms/addClient/addClient.xlsx
+++ b/app/tables/femaleClients/forms/addClient/addClient.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="31100" yWindow="1060" windowWidth="25600" windowHeight="16020" tabRatio="500"/>
+    <workbookView xWindow="1120" yWindow="0" windowWidth="25600" windowHeight="16080" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="choices" sheetId="2" r:id="rId2"/>
     <sheet name="settings" sheetId="3" r:id="rId3"/>
+    <sheet name="model" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="109">
   <si>
     <t>type</t>
   </si>
@@ -151,6 +152,204 @@
   </si>
   <si>
     <t>display.hint</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>interviewer_id</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>delivery_date</t>
+  </si>
+  <si>
+    <t>baby_alive</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>baby_weight</t>
+  </si>
+  <si>
+    <t>baby_alive_now</t>
+  </si>
+  <si>
+    <t>baby_weight_now</t>
+  </si>
+  <si>
+    <t>delivery_location_other</t>
+  </si>
+  <si>
+    <t>delivery_assisted</t>
+  </si>
+  <si>
+    <t>delivery_assisted_other</t>
+  </si>
+  <si>
+    <t>induced_labor</t>
+  </si>
+  <si>
+    <t>c_section</t>
+  </si>
+  <si>
+    <t>select_multiple</t>
+  </si>
+  <si>
+    <t>complications</t>
+  </si>
+  <si>
+    <t>complications_other</t>
+  </si>
+  <si>
+    <t>bf_after_deliv</t>
+  </si>
+  <si>
+    <t>still_bf</t>
+  </si>
+  <si>
+    <t>bf_duration</t>
+  </si>
+  <si>
+    <t>hiv_tested</t>
+  </si>
+  <si>
+    <t>test_location</t>
+  </si>
+  <si>
+    <t>test_location_other</t>
+  </si>
+  <si>
+    <t>test_result</t>
+  </si>
+  <si>
+    <t>ccc</t>
+  </si>
+  <si>
+    <t>cd4_known</t>
+  </si>
+  <si>
+    <t>cd4_count</t>
+  </si>
+  <si>
+    <t>prescr_meds</t>
+  </si>
+  <si>
+    <t>art</t>
+  </si>
+  <si>
+    <t>azt</t>
+  </si>
+  <si>
+    <t>art_duration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one </t>
+  </si>
+  <si>
+    <t>art_curr</t>
+  </si>
+  <si>
+    <t>labor_meds</t>
+  </si>
+  <si>
+    <t>meds_after_deliv</t>
+  </si>
+  <si>
+    <t>child_meds</t>
+  </si>
+  <si>
+    <t>child_curr_meds</t>
+  </si>
+  <si>
+    <t>child_missed_doses</t>
+  </si>
+  <si>
+    <t>rel_change</t>
+  </si>
+  <si>
+    <t>rel_change_other</t>
+  </si>
+  <si>
+    <t>rel_end_study</t>
+  </si>
+  <si>
+    <t>rel_end_reason</t>
+  </si>
+  <si>
+    <t>Rel_OtherEnd</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>delivery_location</t>
+  </si>
+  <si>
+    <t>infant_test</t>
+  </si>
+  <si>
+    <t>agree_screening</t>
+  </si>
+  <si>
+    <t>pregnant</t>
+  </si>
+  <si>
+    <t>gestational_age</t>
+  </si>
+  <si>
+    <t>ethnic_group</t>
+  </si>
+  <si>
+    <t>ethnic_group_other</t>
+  </si>
+  <si>
+    <t>education_level</t>
+  </si>
+  <si>
+    <t>religion</t>
+  </si>
+  <si>
+    <t>religion_other</t>
+  </si>
+  <si>
+    <t>employment</t>
+  </si>
+  <si>
+    <t>employment_other</t>
+  </si>
+  <si>
+    <t>curr_relationship</t>
+  </si>
+  <si>
+    <t>partner_age</t>
+  </si>
+  <si>
+    <t>times_pregnant</t>
+  </si>
+  <si>
+    <t>living_children</t>
+  </si>
+  <si>
+    <t>clinic_proximity</t>
+  </si>
+  <si>
+    <t>client_consent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_multiple </t>
+  </si>
+  <si>
+    <t>refusal_reasons</t>
+  </si>
+  <si>
+    <t>refusal_reasons_other</t>
+  </si>
+  <si>
+    <t>interviewer_init</t>
   </si>
 </sst>
 </file>
@@ -189,7 +388,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,6 +405,30 @@
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDAEEF3"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDA9694"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC4D79B"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -242,7 +465,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="519">
+  <cellStyleXfs count="597">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -762,8 +985,86 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -810,8 +1111,24 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="519">
+  <cellStyles count="597">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1071,6 +1388,45 @@
     <cellStyle name="Followed Hyperlink" xfId="514" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="516" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="518" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="520" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="522" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="524" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="526" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="528" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="530" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="532" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="534" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="536" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="538" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="540" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="542" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="544" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="546" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="548" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="550" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="552" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="554" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="556" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="558" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="560" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="562" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="564" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="566" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="568" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="570" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="572" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="574" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="576" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="578" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="580" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="582" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="584" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="586" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="588" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="590" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="592" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="594" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="596" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1330,6 +1686,45 @@
     <cellStyle name="Hyperlink" xfId="513" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="515" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="517" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="519" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="521" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="523" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="525" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="527" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="529" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="531" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="533" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="535" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="537" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="539" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="541" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="543" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="545" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="547" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="549" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="551" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="553" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="555" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="557" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="559" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="561" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="563" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="565" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="567" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="569" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="571" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="573" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="575" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="577" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="579" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="581" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="583" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="585" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="587" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="589" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="591" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="593" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="595" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1666,11 +2061,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1934,4 +2329,550 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="30.83203125" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="32" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" s="19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" s="19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B47" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B48" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B49" s="21" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B50" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B51" s="21" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B52" s="21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B53" s="21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B54" s="21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B55" s="21" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B56" s="21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B57" s="21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B58" s="21" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B59" s="21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B60" s="21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B61" s="21" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B62" s="21" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B63" s="21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="B64" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B65" s="21" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>